<commit_message>
- fixed : search highlight html entities with empty search - fixed : search bar debounce sync highlight and result - fixed : search bar remove recent search btn - fixed : search bar colspan diff with recent search - added : modality description in table modalities
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428104CD-03CC-FE45-83C6-ECD9391DBBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20757F5-86B9-0044-A3DA-66AA5C3502C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>closed_data</t>
   </si>
   <si>
-    <t>description of dataset 3</t>
-  </si>
-  <si>
     <t>month</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>csv</t>
+  </si>
+  <si>
+    <t>description of dataset 3, with speacial html l'ike &gt; or &amp; or &lt; d'es fois</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -588,22 +588,22 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
         <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
         <v>8</v>
       </c>
       <c r="P1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -641,10 +641,10 @@
         <v>2023</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -673,28 +673,28 @@
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -717,21 +717,21 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="H4">
         <v>3001</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed : remove errors when dataset has no folder or institution, added : demo dataset with lot of variable to test datatables scroller, changed : dont make static page for variable and modality
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20757F5-86B9-0044-A3DA-66AA5C3502C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256743A4-4A67-1349-948E-37F34FE161D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>description of dataset 3, with speacial html l'ike &gt; or &amp; or &lt; d'es fois</t>
+  </si>
+  <si>
+    <t>a dataset with a lot of variables</t>
+  </si>
+  <si>
+    <t>dataset_4</t>
+  </si>
+  <si>
+    <t>dataset with lot of variables</t>
   </si>
 </sst>
 </file>
@@ -221,8 +230,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:P4" totalsRowShown="0">
-  <autoFilter ref="A1:P4" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:P5" totalsRowShown="0">
+  <autoFilter ref="A1:P5" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{080E2F00-A22C-534D-B9C4-D8C8D5EB31DA}" name="id"/>
     <tableColumn id="2" xr3:uid="{92BFA972-4C1D-4E43-B990-63C7415BF3D0}" name="folder_id"/>
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -544,9 +553,9 @@
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
@@ -554,6 +563,7 @@
     <col min="12" max="13" width="12.5" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -733,6 +743,25 @@
       <c r="N4" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
changed : make demo data more realistic and complete
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256743A4-4A67-1349-948E-37F34FE161D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E04327A-3FDF-7C4C-9B56-928A6B287AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="115">
   <si>
     <t>id</t>
   </si>
@@ -61,66 +61,9 @@
     <t>open_data</t>
   </si>
   <si>
-    <t>dataset_1</t>
-  </si>
-  <si>
-    <t>folder_2</t>
-  </si>
-  <si>
-    <t>institution_1</t>
-  </si>
-  <si>
-    <t>institution_3</t>
-  </si>
-  <si>
-    <t>dataset 1</t>
-  </si>
-  <si>
-    <t>description of dataset 1</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>dataset_2</t>
-  </si>
-  <si>
-    <t>folder_3</t>
-  </si>
-  <si>
-    <t>dataset 2</t>
-  </si>
-  <si>
-    <t>description of dataset 2</t>
-  </si>
-  <si>
-    <t>institution_2</t>
-  </si>
-  <si>
-    <t>dataset_3</t>
-  </si>
-  <si>
-    <t>dataset 3</t>
-  </si>
-  <si>
     <t>closed_data</t>
   </si>
   <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>swiss</t>
-  </si>
-  <si>
-    <t>germany</t>
-  </si>
-  <si>
-    <t>france</t>
-  </si>
-  <si>
-    <t>2023/10/22</t>
-  </si>
-  <si>
     <t>data/dataset/dataset_2.xlsx</t>
   </si>
   <si>
@@ -148,16 +91,280 @@
     <t>csv</t>
   </si>
   <si>
-    <t>description of dataset 3, with speacial html l'ike &gt; or &amp; or &lt; d'es fois</t>
-  </si>
-  <si>
-    <t>a dataset with a lot of variables</t>
-  </si>
-  <si>
-    <t>dataset_4</t>
-  </si>
-  <si>
-    <t>dataset with lot of variables</t>
+    <t>Données sur les services publics locaux</t>
+  </si>
+  <si>
+    <t>Services publics locaux</t>
+  </si>
+  <si>
+    <t>année</t>
+  </si>
+  <si>
+    <t>mois</t>
+  </si>
+  <si>
+    <t>Genève</t>
+  </si>
+  <si>
+    <t>Suisse</t>
+  </si>
+  <si>
+    <t>Valais</t>
+  </si>
+  <si>
+    <t>ser_pub_loc</t>
+  </si>
+  <si>
+    <t>Statistiques des accidents de la route</t>
+  </si>
+  <si>
+    <t>Accidents de la route</t>
+  </si>
+  <si>
+    <t>accident_route</t>
+  </si>
+  <si>
+    <t>Analyse des dépenses publiques en santé</t>
+  </si>
+  <si>
+    <t>2024/10/01</t>
+  </si>
+  <si>
+    <t>2023/04/22</t>
+  </si>
+  <si>
+    <t>Dépenses publiques en santé</t>
+  </si>
+  <si>
+    <t>dep_sante</t>
+  </si>
+  <si>
+    <t>Évolution des températures moyennes mensuelles</t>
+  </si>
+  <si>
+    <t>Températures moyennes</t>
+  </si>
+  <si>
+    <t>temperature_moy</t>
+  </si>
+  <si>
+    <t>sas</t>
+  </si>
+  <si>
+    <t>pop_region</t>
+  </si>
+  <si>
+    <t>Population par région</t>
+  </si>
+  <si>
+    <t>Données démographiques par région</t>
+  </si>
+  <si>
+    <t>2024/09/15</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>eco_energies</t>
+  </si>
+  <si>
+    <t>Économie des énergies renouvelables</t>
+  </si>
+  <si>
+    <t>Étude sur l’impact économique des énergies renouvelables</t>
+  </si>
+  <si>
+    <t>2024/06/11</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>eau_potable</t>
+  </si>
+  <si>
+    <t>Qualité de l’eau potable</t>
+  </si>
+  <si>
+    <t>Données sur la qualité de l’eau potable dans différentes régions</t>
+  </si>
+  <si>
+    <t>2023/12/20</t>
+  </si>
+  <si>
+    <t>2010</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>tourisme_annu</t>
+  </si>
+  <si>
+    <t>Statistiques du tourisme annuel</t>
+  </si>
+  <si>
+    <t>Statistiques des arrivées et nuitées dans les établissements touristiques</t>
+  </si>
+  <si>
+    <t>2024/09/30</t>
+  </si>
+  <si>
+    <t>trimestre</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>pollution_air</t>
+  </si>
+  <si>
+    <t>Taux de pollution de l’air</t>
+  </si>
+  <si>
+    <t>Données sur la pollution de l’air en zone urbaine</t>
+  </si>
+  <si>
+    <t>2024/07/15</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>Suisse romande</t>
+  </si>
+  <si>
+    <t>Vaud</t>
+  </si>
+  <si>
+    <t>transport_pub</t>
+  </si>
+  <si>
+    <t>Fréquentation des transports publics</t>
+  </si>
+  <si>
+    <t>Données sur la fréquentation des transports publics par ville</t>
+  </si>
+  <si>
+    <t>2024/09/01</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>usage_internet</t>
+  </si>
+  <si>
+    <t>Usage d’internet par âge</t>
+  </si>
+  <si>
+    <t>Statistiques d’utilisation d’internet selon les tranches d’âge</t>
+  </si>
+  <si>
+    <t>2024/05/12</t>
+  </si>
+  <si>
+    <t>emplois_tech</t>
+  </si>
+  <si>
+    <t>Évolution des emplois dans la tech</t>
+  </si>
+  <si>
+    <t>Analyse de la croissance des emplois dans le secteur technologique</t>
+  </si>
+  <si>
+    <t>2024/02/19</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>accidents_travail</t>
+  </si>
+  <si>
+    <t>Accidents du travail</t>
+  </si>
+  <si>
+    <t>Statistiques des accidents du travail par secteur</t>
+  </si>
+  <si>
+    <t>2023/11/05</t>
+  </si>
+  <si>
+    <t>vente_voitures</t>
+  </si>
+  <si>
+    <t>Ventes de voitures neuves</t>
+  </si>
+  <si>
+    <t>Statistiques des ventes de voitures neuves par région</t>
+  </si>
+  <si>
+    <t>2024/08/25</t>
+  </si>
+  <si>
+    <t>exportations</t>
+  </si>
+  <si>
+    <t>Exportations suisses</t>
+  </si>
+  <si>
+    <t>Données sur les exportations suisses par secteur</t>
+  </si>
+  <si>
+    <t>2024/07/10</t>
+  </si>
+  <si>
+    <t>immobilier_prix</t>
+  </si>
+  <si>
+    <t>Évolution des prix immobiliers</t>
+  </si>
+  <si>
+    <t>Analyse des prix de l’immobilier dans les grandes villes</t>
+  </si>
+  <si>
+    <t>2024/09/25</t>
+  </si>
+  <si>
+    <t>conso_energie</t>
+  </si>
+  <si>
+    <t>Consommation d’énergie par secteur</t>
+  </si>
+  <si>
+    <t>Données sur la consommation d’énergie selon le secteur économique</t>
+  </si>
+  <si>
+    <t>revenus_menages</t>
+  </si>
+  <si>
+    <t>Revenus des ménages</t>
+  </si>
+  <si>
+    <t>Étude sur les revenus des ménages suisses</t>
+  </si>
+  <si>
+    <t>2024/06/30</t>
+  </si>
+  <si>
+    <t>emploi_jeunes</t>
+  </si>
+  <si>
+    <t>Taux d’emploi des jeunes</t>
+  </si>
+  <si>
+    <t>Données sur l’emploi des jeunes de 18 à 25 ans</t>
+  </si>
+  <si>
+    <t>2024/09/10</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
 </sst>
 </file>
@@ -230,8 +437,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:P5" totalsRowShown="0">
-  <autoFilter ref="A1:P5" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:P20" totalsRowShown="0">
+  <autoFilter ref="A1:P20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{080E2F00-A22C-534D-B9C4-D8C8D5EB31DA}" name="id"/>
     <tableColumn id="2" xr3:uid="{92BFA972-4C1D-4E43-B990-63C7415BF3D0}" name="folder_id"/>
@@ -541,26 +748,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
@@ -598,51 +806,42 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s">
         <v>8</v>
       </c>
       <c r="P1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2">
         <v>3000</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1">
         <v>2002</v>
@@ -651,117 +850,633 @@
         <v>2023</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H3">
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="N3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="O3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4">
+        <v>43023</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
         <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4">
-        <v>3001</v>
-      </c>
-      <c r="J4" t="s">
-        <v>28</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H5">
         <v>200</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6">
+        <v>500000</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7">
+        <v>10235</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8">
+        <v>80000</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" t="s">
+        <v>71</v>
+      </c>
+      <c r="N8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9">
+        <v>320000</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10">
+        <v>67000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11">
+        <v>90000</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12">
+        <v>500000</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13">
+        <v>200000</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14">
+        <v>85000</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15">
+        <v>120000</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J15" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16">
+        <v>250000</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17">
+        <v>100000</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" t="s">
+        <v>71</v>
+      </c>
+      <c r="N17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>105</v>
+      </c>
+      <c r="H18">
+        <v>300000</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M18" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19">
+        <v>45000</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" t="s">
+        <v>72</v>
+      </c>
+      <c r="N19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20">
+        <v>100000</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
changed : denormalize db schema to remove many to many relation table
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E04327A-3FDF-7C4C-9B56-928A6B287AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A781AB-21D6-3442-BE71-3E9E0AD24CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -365,6 +365,21 @@
   </si>
   <si>
     <t>2016</t>
+  </si>
+  <si>
+    <t>doc_ids</t>
+  </si>
+  <si>
+    <t>pdf_wiki, pdf_online</t>
+  </si>
+  <si>
+    <t>tag_ids</t>
+  </si>
+  <si>
+    <t>personal_data, sensible_data, sante, population</t>
+  </si>
+  <si>
+    <t>anonymous_data, population, culture</t>
   </si>
 </sst>
 </file>
@@ -406,9 +421,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,9 +455,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:P20" totalsRowShown="0">
-  <autoFilter ref="A1:P20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:R20" totalsRowShown="0">
+  <autoFilter ref="A1:R20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
+  <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{080E2F00-A22C-534D-B9C4-D8C8D5EB31DA}" name="id"/>
     <tableColumn id="2" xr3:uid="{92BFA972-4C1D-4E43-B990-63C7415BF3D0}" name="folder_id"/>
     <tableColumn id="3" xr3:uid="{39D90AAB-DB99-4842-B7A2-ED8697C478CE}" name="owner_id"/>
@@ -456,6 +474,8 @@
     <tableColumn id="16" xr3:uid="{ED3587E2-4956-D94E-81CF-A84E6EFAC119}" name="delivery_format"/>
     <tableColumn id="14" xr3:uid="{7536954D-F305-F647-B54D-43D736B0B7C6}" name="link"/>
     <tableColumn id="15" xr3:uid="{E59E90FD-B1FC-204A-B6BB-8501C30CA936}" name="data_path"/>
+    <tableColumn id="18" xr3:uid="{4730D97E-AE17-A44B-9512-0BF292D5AFB4}" name="tag_ids"/>
+    <tableColumn id="19" xr3:uid="{288E2992-818F-AA4B-8F92-E9D2F7E670E8}" name="doc_ids"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -748,10 +768,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -772,9 +795,11 @@
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -823,8 +848,14 @@
       <c r="P1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -856,7 +887,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -897,7 +928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -927,8 +958,14 @@
       <c r="N4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="R4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -953,7 +990,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -988,7 +1025,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1023,7 +1060,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1058,7 +1095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1093,7 +1130,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1128,7 +1165,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -1163,7 +1200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1197,8 +1234,11 @@
       <c r="N12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -1233,7 +1273,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1268,7 +1308,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -1303,7 +1343,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
fixed : ellipsis on extendable tree on entity info page
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A781AB-21D6-3442-BE71-3E9E0AD24CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1487199C-6C42-0B46-8ABE-ED700AE2E6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -771,10 +771,10 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1322,7 @@
         <v>93</v>
       </c>
       <c r="H15">
-        <v>120000</v>
+        <v>99900</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>94</v>
@@ -1427,7 +1427,7 @@
         <v>105</v>
       </c>
       <c r="H18">
-        <v>300000</v>
+        <v>1300000</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
fixed : sort by dataset nb line as numeric even if empty value
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1487199C-6C42-0B46-8ABE-ED700AE2E6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBB1906-2D30-5146-A497-AFD9E6C09D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,7 +774,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1038,9 +1038,6 @@
       <c r="G7" t="s">
         <v>51</v>
       </c>
-      <c r="H7">
-        <v>10235</v>
-      </c>
       <c r="I7" s="1" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
added : dataset folder in demo data
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBB1906-2D30-5146-A497-AFD9E6C09D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CF95DB-3D78-324E-BB73-9E3FC5C66695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
   <si>
     <t>id</t>
   </si>
@@ -380,6 +380,54 @@
   </si>
   <si>
     <t>anonymous_data, population, culture</t>
+  </si>
+  <si>
+    <t>14-sante</t>
+  </si>
+  <si>
+    <t>04-economie</t>
+  </si>
+  <si>
+    <t>01-pop</t>
+  </si>
+  <si>
+    <t>03-travail</t>
+  </si>
+  <si>
+    <t>08-energie</t>
+  </si>
+  <si>
+    <t>12-monnaie</t>
+  </si>
+  <si>
+    <t>06-industrie</t>
+  </si>
+  <si>
+    <t>11-mobilite</t>
+  </si>
+  <si>
+    <t>10-tourisme</t>
+  </si>
+  <si>
+    <t>02-espace</t>
+  </si>
+  <si>
+    <t>17-politique</t>
+  </si>
+  <si>
+    <t>ofs-salaire</t>
+  </si>
+  <si>
+    <t>ofs-travail</t>
+  </si>
+  <si>
+    <t>ofs</t>
+  </si>
+  <si>
+    <t>ofs-tourisme</t>
+  </si>
+  <si>
+    <t>ofs-div-pop</t>
   </si>
 </sst>
 </file>
@@ -771,10 +819,10 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -783,7 +831,7 @@
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
@@ -859,6 +907,9 @@
       <c r="A2" t="s">
         <v>30</v>
       </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
       <c r="E2" t="s">
         <v>24</v>
       </c>
@@ -891,6 +942,9 @@
       <c r="A3" t="s">
         <v>33</v>
       </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
@@ -931,6 +985,9 @@
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
@@ -969,6 +1026,9 @@
       <c r="A5" t="s">
         <v>41</v>
       </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
       <c r="E5" t="s">
         <v>40</v>
       </c>
@@ -994,6 +1054,15 @@
       <c r="A6" t="s">
         <v>43</v>
       </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
+        <v>135</v>
+      </c>
       <c r="E6" t="s">
         <v>44</v>
       </c>
@@ -1029,6 +1098,9 @@
       <c r="A7" t="s">
         <v>49</v>
       </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
       <c r="E7" t="s">
         <v>50</v>
       </c>
@@ -1061,6 +1133,9 @@
       <c r="A8" t="s">
         <v>54</v>
       </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
       <c r="E8" t="s">
         <v>55</v>
       </c>
@@ -1096,6 +1171,15 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
+      <c r="B9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
       <c r="E9" t="s">
         <v>61</v>
       </c>
@@ -1131,6 +1215,9 @@
       <c r="A10" t="s">
         <v>66</v>
       </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
       <c r="E10" t="s">
         <v>67</v>
       </c>
@@ -1166,6 +1253,9 @@
       <c r="A11" t="s">
         <v>73</v>
       </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
       <c r="E11" t="s">
         <v>74</v>
       </c>
@@ -1201,6 +1291,9 @@
       <c r="A12" t="s">
         <v>78</v>
       </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
       <c r="E12" t="s">
         <v>79</v>
       </c>
@@ -1239,6 +1332,9 @@
       <c r="A13" t="s">
         <v>82</v>
       </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
       <c r="E13" t="s">
         <v>83</v>
       </c>
@@ -1274,6 +1370,9 @@
       <c r="A14" t="s">
         <v>87</v>
       </c>
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
       <c r="E14" t="s">
         <v>88</v>
       </c>
@@ -1309,6 +1408,9 @@
       <c r="A15" t="s">
         <v>91</v>
       </c>
+      <c r="B15" t="s">
+        <v>127</v>
+      </c>
       <c r="E15" t="s">
         <v>92</v>
       </c>
@@ -1344,6 +1446,9 @@
       <c r="A16" t="s">
         <v>95</v>
       </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
       <c r="E16" t="s">
         <v>96</v>
       </c>
@@ -1379,6 +1484,9 @@
       <c r="A17" t="s">
         <v>99</v>
       </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
       <c r="E17" t="s">
         <v>100</v>
       </c>
@@ -1414,6 +1522,9 @@
       <c r="A18" t="s">
         <v>103</v>
       </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
       <c r="E18" t="s">
         <v>104</v>
       </c>
@@ -1449,6 +1560,15 @@
       <c r="A19" t="s">
         <v>106</v>
       </c>
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" t="s">
+        <v>131</v>
+      </c>
       <c r="E19" t="s">
         <v>107</v>
       </c>
@@ -1483,6 +1603,15 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>110</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
       </c>
       <c r="E20" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
added : column nb variable for institutions and folders
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CF95DB-3D78-324E-BB73-9E3FC5C66695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330E67E0-3E1E-804B-B889-2ED42742F830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="136">
   <si>
     <t>id</t>
   </si>
@@ -822,7 +822,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -910,6 +910,12 @@
       <c r="B2" t="s">
         <v>130</v>
       </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
       <c r="E2" t="s">
         <v>24</v>
       </c>
@@ -945,6 +951,12 @@
       <c r="B3" t="s">
         <v>127</v>
       </c>
+      <c r="C3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
@@ -988,6 +1000,12 @@
       </c>
       <c r="B4" t="s">
         <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
added : history diff with highlight of delete and add on row and value
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330E67E0-3E1E-804B-B889-2ED42742F830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD8BC4F-4341-F44A-9AFE-2063CD286F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>dep_sante</t>
   </si>
   <si>
-    <t>Évolution des températures moyennes mensuelles</t>
-  </si>
-  <si>
     <t>Températures moyennes</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Population par région</t>
   </si>
   <si>
-    <t>Données démographiques par région</t>
-  </si>
-  <si>
     <t>2024/09/15</t>
   </si>
   <si>
@@ -325,9 +319,6 @@
     <t>Évolution des prix immobiliers</t>
   </si>
   <si>
-    <t>Analyse des prix de l’immobilier dans les grandes villes</t>
-  </si>
-  <si>
     <t>2024/09/25</t>
   </si>
   <si>
@@ -428,6 +419,15 @@
   </si>
   <si>
     <t>ofs-div-pop</t>
+  </si>
+  <si>
+    <t>Données démographiques et géographiques par région</t>
+  </si>
+  <si>
+    <t>Évolution des températures mensuelles</t>
+  </si>
+  <si>
+    <t>Analyse des prix des biens immobiliers dans les grandes villes</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -897,10 +897,10 @@
         <v>19</v>
       </c>
       <c r="Q1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="R1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -908,13 +908,13 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
         <v>130</v>
       </c>
-      <c r="C2" t="s">
-        <v>133</v>
-      </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -949,13 +949,13 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -999,13 +999,13 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
@@ -1034,27 +1034,27 @@
         <v>22</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="R4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1065,45 +1065,45 @@
         <v>29</v>
       </c>
       <c r="N5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="H6">
         <v>500000</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M6" t="s">
         <v>28</v>
@@ -1114,31 +1114,31 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J7" t="s">
         <v>26</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M7" t="s">
         <v>27</v>
@@ -1149,37 +1149,37 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H8">
         <v>80000</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J8" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N8" t="s">
         <v>22</v>
@@ -1187,81 +1187,81 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H9">
         <v>320000</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M9" t="s">
         <v>28</v>
       </c>
       <c r="N9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H10">
         <v>67000</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J10" t="s">
         <v>26</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" t="s">
         <v>70</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" t="s">
-        <v>72</v>
       </c>
       <c r="N10" t="s">
         <v>22</v>
@@ -1269,34 +1269,34 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
         <v>73</v>
-      </c>
-      <c r="B11" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>75</v>
       </c>
       <c r="H11">
         <v>90000</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J11" t="s">
         <v>26</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M11" t="s">
         <v>29</v>
@@ -1307,34 +1307,34 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H12">
         <v>500000</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J12" t="s">
         <v>25</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M12" t="s">
         <v>28</v>
@@ -1343,39 +1343,39 @@
         <v>21</v>
       </c>
       <c r="Q12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H13">
         <v>200000</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M13" t="s">
         <v>27</v>
@@ -1386,72 +1386,72 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H14">
         <v>85000</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J14" t="s">
         <v>25</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
         <v>29</v>
       </c>
       <c r="N14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H15">
         <v>99900</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M15" t="s">
         <v>28</v>
@@ -1462,34 +1462,34 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H16">
         <v>250000</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J16" t="s">
         <v>26</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M16" t="s">
         <v>27</v>
@@ -1500,37 +1500,37 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="H17">
         <v>100000</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N17" t="s">
         <v>22</v>
@@ -1538,81 +1538,81 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H18">
         <v>1300000</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J18" t="s">
         <v>26</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M18" t="s">
         <v>28</v>
       </c>
       <c r="N18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H19">
         <v>45000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J19" t="s">
         <v>25</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N19" t="s">
         <v>22</v>
@@ -1620,40 +1620,40 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M20" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
added : history parent entity column
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD8BC4F-4341-F44A-9AFE-2063CD286F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293597B4-4DD1-7840-A49E-4D1516FDFC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,9 +265,6 @@
     <t>emplois_tech</t>
   </si>
   <si>
-    <t>Évolution des emplois dans la tech</t>
-  </si>
-  <si>
     <t>Analyse de la croissance des emplois dans le secteur technologique</t>
   </si>
   <si>
@@ -428,6 +425,9 @@
   </si>
   <si>
     <t>Analyse des prix des biens immobiliers dans les grandes villes</t>
+  </si>
+  <si>
+    <t>Évolution des emplois dans la tech et l'IT</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -897,10 +897,10 @@
         <v>19</v>
       </c>
       <c r="Q1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -908,13 +908,13 @@
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
         <v>130</v>
-      </c>
-      <c r="D2" t="s">
-        <v>131</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -949,13 +949,13 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -999,13 +999,13 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
         <v>37</v>
@@ -1034,10 +1034,10 @@
         <v>22</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -1045,7 +1045,7 @@
         <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
         <v>39</v>
@@ -1054,7 +1054,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1073,13 +1073,13 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
@@ -1088,7 +1088,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1117,7 +1117,7 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
         <v>48</v>
@@ -1152,7 +1152,7 @@
         <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E8" t="s">
         <v>53</v>
@@ -1190,13 +1190,13 @@
         <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
         <v>130</v>
-      </c>
-      <c r="D9" t="s">
-        <v>131</v>
       </c>
       <c r="E9" t="s">
         <v>59</v>
@@ -1234,7 +1234,7 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E10" t="s">
         <v>65</v>
@@ -1272,7 +1272,7 @@
         <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
         <v>72</v>
@@ -1310,7 +1310,7 @@
         <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
         <v>77</v>
@@ -1343,7 +1343,7 @@
         <v>21</v>
       </c>
       <c r="Q12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -1351,28 +1351,28 @@
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13">
         <v>200000</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" t="s">
         <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>46</v>
@@ -1386,25 +1386,25 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" t="s">
         <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" t="s">
-        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H14">
         <v>85000</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J14" t="s">
         <v>25</v>
@@ -1424,25 +1424,25 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E15" t="s">
         <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" t="s">
-        <v>90</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H15">
         <v>99900</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J15" t="s">
         <v>62</v>
@@ -1462,25 +1462,25 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" t="s">
         <v>93</v>
-      </c>
-      <c r="B16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" t="s">
-        <v>94</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H16">
         <v>250000</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J16" t="s">
         <v>26</v>
@@ -1500,25 +1500,25 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" t="s">
         <v>97</v>
-      </c>
-      <c r="B17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" t="s">
-        <v>98</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H17">
         <v>100000</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
@@ -1538,19 +1538,19 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" t="s">
         <v>100</v>
-      </c>
-      <c r="B18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" t="s">
-        <v>101</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H18">
         <v>1300000</v>
@@ -1576,31 +1576,31 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" t="s">
         <v>103</v>
-      </c>
-      <c r="B19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" t="s">
-        <v>128</v>
-      </c>
-      <c r="E19" t="s">
-        <v>104</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H19">
         <v>45000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J19" t="s">
         <v>25</v>
@@ -1620,37 +1620,37 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E20" t="s">
         <v>107</v>
-      </c>
-      <c r="B20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" t="s">
-        <v>108</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J20" t="s">
         <v>62</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
added : history validity start, end and update date and next_update_date estimation
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293597B4-4DD1-7840-A49E-4D1516FDFC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B211D-D6B3-F343-A6D1-7AC9113C5EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="141">
   <si>
     <t>id</t>
   </si>
@@ -97,12 +97,6 @@
     <t>Services publics locaux</t>
   </si>
   <si>
-    <t>année</t>
-  </si>
-  <si>
-    <t>mois</t>
-  </si>
-  <si>
     <t>Genève</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
     <t>2024/09/30</t>
   </si>
   <si>
-    <t>trimestre</t>
-  </si>
-  <si>
     <t>2015</t>
   </si>
   <si>
@@ -241,9 +232,6 @@
     <t>Fréquentation des transports publics</t>
   </si>
   <si>
-    <t>Données sur la fréquentation des transports publics par ville</t>
-  </si>
-  <si>
     <t>2024/09/01</t>
   </si>
   <si>
@@ -428,6 +416,33 @@
   </si>
   <si>
     <t>Évolution des emplois dans la tech et l'IT</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>2026</t>
+  </si>
+  <si>
+    <t>annuelle</t>
+  </si>
+  <si>
+    <t>mensuelle</t>
+  </si>
+  <si>
+    <t>trimestrielle</t>
+  </si>
+  <si>
+    <t>semestrielle</t>
+  </si>
+  <si>
+    <t>Données sur les transports publics par ville et village</t>
+  </si>
+  <si>
+    <t>emplois_tech2</t>
+  </si>
+  <si>
+    <t>Évolution des emplois de la tech</t>
   </si>
 </sst>
 </file>
@@ -816,13 +831,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -897,24 +912,24 @@
         <v>19</v>
       </c>
       <c r="Q1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="R1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
         <v>126</v>
-      </c>
-      <c r="C2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -929,7 +944,7 @@
         <v>3000</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="K2" s="1">
         <v>2002</v>
@@ -938,7 +953,7 @@
         <v>2023</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
         <v>22</v>
@@ -946,34 +961,34 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3">
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>17</v>
@@ -982,7 +997,7 @@
         <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
         <v>21</v>
@@ -996,65 +1011,65 @@
     </row>
     <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4">
         <v>43023</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
         <v>22</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="R4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1062,51 +1077,51 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H6">
         <v>500000</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="M6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s">
         <v>22</v>
@@ -1114,34 +1129,34 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" t="s">
+        <v>135</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N7" t="s">
         <v>21</v>
@@ -1149,37 +1164,37 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>80000</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="M8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N8" t="s">
         <v>22</v>
@@ -1187,81 +1202,81 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H9">
         <v>320000</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J9" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H10">
         <v>67000</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" t="s">
+        <v>135</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" t="s">
         <v>67</v>
-      </c>
-      <c r="J10" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" t="s">
-        <v>70</v>
       </c>
       <c r="N10" t="s">
         <v>22</v>
@@ -1269,37 +1284,37 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="H11">
         <v>90000</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N11" t="s">
         <v>22</v>
@@ -1307,78 +1322,78 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H12">
         <v>500000</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>46</v>
+        <v>132</v>
       </c>
       <c r="M12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="Q12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H13">
         <v>200000</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N13" t="s">
         <v>22</v>
@@ -1386,75 +1401,75 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H14">
         <v>85000</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H15">
         <v>99900</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N15" t="s">
         <v>22</v>
@@ -1462,37 +1477,37 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H16">
         <v>250000</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J16" t="s">
-        <v>26</v>
+        <v>135</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
         <v>21</v>
@@ -1500,37 +1515,37 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H17">
         <v>100000</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N17" t="s">
         <v>22</v>
@@ -1538,81 +1553,81 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H18">
         <v>1300000</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J18" t="s">
+        <v>135</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" t="s">
         <v>26</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" t="s">
-        <v>28</v>
-      </c>
       <c r="N18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H19">
         <v>45000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="N19" t="s">
         <v>22</v>
@@ -1620,45 +1635,83 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J20" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21">
+        <v>200000</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" t="s">
+        <v>136</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N21" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed : history hide column time
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B211D-D6B3-F343-A6D1-7AC9113C5EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4726EDAE-BD0D-5049-8ABB-889AA8FF8971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="143">
   <si>
     <t>id</t>
   </si>
@@ -331,9 +331,6 @@
     <t>emploi_jeunes</t>
   </si>
   <si>
-    <t>Taux d’emploi des jeunes</t>
-  </si>
-  <si>
     <t>Données sur l’emploi des jeunes de 18 à 25 ans</t>
   </si>
   <si>
@@ -443,6 +440,15 @@
   </si>
   <si>
     <t>Évolution des emplois de la tech</t>
+  </si>
+  <si>
+    <t>archived</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Taux d’emploi des jeunes et des moins jeunes</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -518,9 +527,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:R20" totalsRowShown="0">
-  <autoFilter ref="A1:R20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
-  <tableColumns count="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:S20" totalsRowShown="0">
+  <autoFilter ref="A1:S20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{080E2F00-A22C-534D-B9C4-D8C8D5EB31DA}" name="id"/>
     <tableColumn id="2" xr3:uid="{92BFA972-4C1D-4E43-B990-63C7415BF3D0}" name="folder_id"/>
     <tableColumn id="3" xr3:uid="{39D90AAB-DB99-4842-B7A2-ED8697C478CE}" name="owner_id"/>
@@ -529,10 +538,11 @@
     <tableColumn id="6" xr3:uid="{D2392623-916B-E04B-A27E-0D01B8B20172}" name="type"/>
     <tableColumn id="7" xr3:uid="{4D4990DC-E580-924E-A6C8-71E0E49DC440}" name="description"/>
     <tableColumn id="8" xr3:uid="{489A14B1-8FC8-C549-8AE1-29C457B8AA01}" name="nb_row"/>
-    <tableColumn id="11" xr3:uid="{39B5740A-29A3-4149-AEFD-550E62863529}" name="last_update_date" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{39B5740A-29A3-4149-AEFD-550E62863529}" name="last_update_date" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{40840879-BBAB-7248-8755-9023914314E8}" name="archived" dataDxfId="0"/>
     <tableColumn id="12" xr3:uid="{25BA5CC3-7EA6-8F48-BADD-686749A186ED}" name="updating_each"/>
-    <tableColumn id="13" xr3:uid="{48FD3A95-5D63-5842-ADE8-82D53CC7CB3B}" name="start_date" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{E9CC3D9F-3681-CE44-9463-02B41A65AEDA}" name="end_date" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{48FD3A95-5D63-5842-ADE8-82D53CC7CB3B}" name="start_date" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{E9CC3D9F-3681-CE44-9463-02B41A65AEDA}" name="end_date" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{AB83C6F1-9210-B442-AD5A-A3BA93064343}" name="localisation"/>
     <tableColumn id="16" xr3:uid="{ED3587E2-4956-D94E-81CF-A84E6EFAC119}" name="delivery_format"/>
     <tableColumn id="14" xr3:uid="{7536954D-F305-F647-B54D-43D736B0B7C6}" name="link"/>
@@ -831,13 +841,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -851,18 +861,19 @@
     <col min="7" max="7" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -890,46 +901,49 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" t="s">
-        <v>109</v>
-      </c>
       <c r="R1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="S1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
         <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>126</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -943,34 +957,34 @@
       <c r="H2">
         <v>3000</v>
       </c>
-      <c r="J2" t="s">
-        <v>134</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="K2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="1">
         <v>2002</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>2023</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -987,40 +1001,43 @@
       <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J3" t="s">
-        <v>134</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>21</v>
-      </c>
-      <c r="O3" t="s">
-        <v>14</v>
       </c>
       <c r="P3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1037,30 +1054,30 @@
       <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J4" t="s">
-        <v>135</v>
-      </c>
-      <c r="K4" s="1"/>
+      <c r="K4" t="s">
+        <v>134</v>
+      </c>
       <c r="L4" s="1"/>
-      <c r="M4" t="s">
+      <c r="M4" s="1"/>
+      <c r="N4" t="s">
         <v>25</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="R4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
@@ -1069,32 +1086,32 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5">
         <v>200</v>
       </c>
-      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" t="s">
+      <c r="M5" s="1"/>
+      <c r="N5" t="s">
         <v>27</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -1103,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1111,28 +1128,28 @@
       <c r="I6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J6" t="s">
-        <v>134</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>26</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -1146,28 +1163,31 @@
       <c r="I7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J7" t="s">
-        <v>135</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>25</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
         <v>51</v>
@@ -1184,34 +1204,34 @@
       <c r="I8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J8" t="s">
-        <v>134</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" t="s">
+        <v>133</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>66</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
         <v>125</v>
-      </c>
-      <c r="D9" t="s">
-        <v>126</v>
       </c>
       <c r="E9" t="s">
         <v>57</v>
@@ -1228,28 +1248,28 @@
       <c r="I9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="J9" t="s">
-        <v>136</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" t="s">
+        <v>135</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
         <v>62</v>
@@ -1266,28 +1286,28 @@
       <c r="I10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J10" t="s">
-        <v>135</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>67</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
         <v>69</v>
@@ -1296,7 +1316,7 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H11">
         <v>90000</v>
@@ -1304,28 +1324,28 @@
       <c r="I11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J11" t="s">
-        <v>135</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>27</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
         <v>73</v>
@@ -1342,34 +1362,34 @@
       <c r="I12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J12" t="s">
-        <v>134</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" t="s">
+        <v>133</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="M12" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="N12" t="s">
         <v>26</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>39</v>
       </c>
-      <c r="Q12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -1383,28 +1403,28 @@
       <c r="I13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J13" t="s">
-        <v>136</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" t="s">
+        <v>135</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="M13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N13" t="s">
         <v>25</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
         <v>81</v>
@@ -1421,28 +1441,28 @@
       <c r="I14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J14" t="s">
-        <v>134</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" t="s">
+        <v>133</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>27</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -1459,28 +1479,28 @@
       <c r="I15" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J15" t="s">
-        <v>136</v>
-      </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" t="s">
+        <v>135</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>26</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" t="s">
         <v>89</v>
@@ -1497,28 +1517,28 @@
       <c r="I16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J16" t="s">
-        <v>135</v>
-      </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>25</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E17" t="s">
         <v>93</v>
@@ -1527,7 +1547,7 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H17">
         <v>100000</v>
@@ -1535,28 +1555,28 @@
       <c r="I17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="J17" t="s">
-        <v>137</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" t="s">
+        <v>136</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>66</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E18" t="s">
         <v>96</v>
@@ -1573,34 +1593,34 @@
       <c r="I18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J18" t="s">
-        <v>135</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>26</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
         <v>99</v>
@@ -1617,75 +1637,75 @@
       <c r="I19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J19" t="s">
-        <v>134</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" t="s">
+        <v>133</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>67</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K20" t="s">
+        <v>135</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J20" t="s">
-        <v>136</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>27</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" t="s">
         <v>139</v>
-      </c>
-      <c r="B21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" t="s">
-        <v>140</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -1699,19 +1719,19 @@
       <c r="I21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J21" t="s">
-        <v>136</v>
-      </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" t="s">
+        <v>135</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="M21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N21" t="s">
         <v>25</v>
       </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added : no_more_update attribute to hide next_update_date
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4726EDAE-BD0D-5049-8ABB-889AA8FF8971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BA43AA-9E06-BF4F-AB57-C030204CDDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -442,13 +442,13 @@
     <t>Évolution des emplois de la tech</t>
   </si>
   <si>
-    <t>archived</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>Taux d’emploi des jeunes et des moins jeunes</t>
+  </si>
+  <si>
+    <t>no_more_update</t>
   </si>
 </sst>
 </file>
@@ -539,10 +539,10 @@
     <tableColumn id="7" xr3:uid="{4D4990DC-E580-924E-A6C8-71E0E49DC440}" name="description"/>
     <tableColumn id="8" xr3:uid="{489A14B1-8FC8-C549-8AE1-29C457B8AA01}" name="nb_row"/>
     <tableColumn id="11" xr3:uid="{39B5740A-29A3-4149-AEFD-550E62863529}" name="last_update_date" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{40840879-BBAB-7248-8755-9023914314E8}" name="archived" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{40840879-BBAB-7248-8755-9023914314E8}" name="no_more_update" dataDxfId="2"/>
     <tableColumn id="12" xr3:uid="{25BA5CC3-7EA6-8F48-BADD-686749A186ED}" name="updating_each"/>
-    <tableColumn id="13" xr3:uid="{48FD3A95-5D63-5842-ADE8-82D53CC7CB3B}" name="start_date" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{E9CC3D9F-3681-CE44-9463-02B41A65AEDA}" name="end_date" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{48FD3A95-5D63-5842-ADE8-82D53CC7CB3B}" name="start_date" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{E9CC3D9F-3681-CE44-9463-02B41A65AEDA}" name="end_date" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{AB83C6F1-9210-B442-AD5A-A3BA93064343}" name="localisation"/>
     <tableColumn id="16" xr3:uid="{ED3587E2-4956-D94E-81CF-A84E6EFAC119}" name="delivery_format"/>
     <tableColumn id="14" xr3:uid="{7536954D-F305-F647-B54D-43D736B0B7C6}" name="link"/>
@@ -844,10 +844,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -860,8 +860,7 @@
     <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.5" customWidth="1"/>
@@ -902,7 +901,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -1002,7 +1001,7 @@
         <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K3" t="s">
         <v>133</v>
@@ -1164,7 +1163,7 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K7" t="s">
         <v>134</v>
@@ -1667,7 +1666,7 @@
         <v>123</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
added : evolution diff for number and date relative
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BA43AA-9E06-BF4F-AB57-C030204CDDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9E3340-9F9F-3543-975E-308420C62B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="144">
   <si>
     <t>id</t>
   </si>
@@ -325,9 +325,6 @@
     <t>Étude sur les revenus des ménages suisses</t>
   </si>
   <si>
-    <t>2024/06/30</t>
-  </si>
-  <si>
     <t>emploi_jeunes</t>
   </si>
   <si>
@@ -449,6 +446,12 @@
   </si>
   <si>
     <t>no_more_update</t>
+  </si>
+  <si>
+    <t>2025/01/19</t>
+  </si>
+  <si>
+    <t>2024/05/30</t>
   </si>
 </sst>
 </file>
@@ -844,10 +847,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,7 +904,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -925,10 +928,10 @@
         <v>19</v>
       </c>
       <c r="R1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -936,13 +939,13 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
         <v>124</v>
-      </c>
-      <c r="D2" t="s">
-        <v>125</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -957,7 +960,7 @@
         <v>3000</v>
       </c>
       <c r="K2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L2" s="1">
         <v>2002</v>
@@ -977,13 +980,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -1001,10 +1004,10 @@
         <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>17</v>
@@ -1030,13 +1033,13 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1054,7 +1057,7 @@
         <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1065,10 +1068,10 @@
         <v>22</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1076,7 +1079,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
@@ -1085,7 +1088,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1104,13 +1107,13 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -1119,7 +1122,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1128,7 +1131,7 @@
         <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>43</v>
@@ -1148,7 +1151,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -1163,10 +1166,10 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>49</v>
@@ -1186,7 +1189,7 @@
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
         <v>51</v>
@@ -1204,7 +1207,7 @@
         <v>53</v>
       </c>
       <c r="K8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>54</v>
@@ -1224,13 +1227,13 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
         <v>124</v>
-      </c>
-      <c r="D9" t="s">
-        <v>125</v>
       </c>
       <c r="E9" t="s">
         <v>57</v>
@@ -1248,7 +1251,7 @@
         <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>60</v>
@@ -1268,7 +1271,7 @@
         <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" t="s">
         <v>62</v>
@@ -1286,7 +1289,7 @@
         <v>64</v>
       </c>
       <c r="K10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>65</v>
@@ -1306,7 +1309,7 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
         <v>69</v>
@@ -1315,7 +1318,7 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H11">
         <v>90000</v>
@@ -1324,7 +1327,7 @@
         <v>70</v>
       </c>
       <c r="K11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>71</v>
@@ -1344,7 +1347,7 @@
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E12" t="s">
         <v>73</v>
@@ -1362,13 +1365,13 @@
         <v>75</v>
       </c>
       <c r="K12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>60</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N12" t="s">
         <v>26</v>
@@ -1377,7 +1380,7 @@
         <v>39</v>
       </c>
       <c r="R12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1385,10 +1388,10 @@
         <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -1403,13 +1406,13 @@
         <v>78</v>
       </c>
       <c r="K13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N13" t="s">
         <v>25</v>
@@ -1423,7 +1426,7 @@
         <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" t="s">
         <v>81</v>
@@ -1441,7 +1444,7 @@
         <v>83</v>
       </c>
       <c r="K14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>54</v>
@@ -1461,7 +1464,7 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -1479,7 +1482,7 @@
         <v>87</v>
       </c>
       <c r="K15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>71</v>
@@ -1499,7 +1502,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E16" t="s">
         <v>89</v>
@@ -1517,7 +1520,7 @@
         <v>91</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>60</v>
@@ -1537,7 +1540,7 @@
         <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
         <v>93</v>
@@ -1546,7 +1549,7 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H17">
         <v>100000</v>
@@ -1555,7 +1558,7 @@
         <v>94</v>
       </c>
       <c r="K17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>54</v>
@@ -1575,7 +1578,7 @@
         <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
         <v>96</v>
@@ -1593,7 +1596,7 @@
         <v>70</v>
       </c>
       <c r="K18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>60</v>
@@ -1613,13 +1616,13 @@
         <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E19" t="s">
         <v>99</v>
@@ -1631,13 +1634,13 @@
         <v>100</v>
       </c>
       <c r="H19">
-        <v>45000</v>
+        <v>46000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="K19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>54</v>
@@ -1654,37 +1657,37 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K20" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="K20" t="s">
-        <v>135</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>44</v>
@@ -1698,13 +1701,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" t="s">
         <v>138</v>
-      </c>
-      <c r="B21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" t="s">
-        <v>139</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -1716,16 +1719,16 @@
         <v>200000</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>78</v>
+        <v>142</v>
       </c>
       <c r="K21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>79</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N21" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
added : evolution diff date format YYYY, YYYYtQ and YYYY/MM
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9E3340-9F9F-3543-975E-308420C62B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB2AE4A-1F9D-9A4B-BAF8-C36A8D3E8335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -169,9 +169,6 @@
     <t>2024/06/11</t>
   </si>
   <si>
-    <t>2019</t>
-  </si>
-  <si>
     <t>eau_potable</t>
   </si>
   <si>
@@ -452,6 +449,18 @@
   </si>
   <si>
     <t>2024/05/30</t>
+  </si>
+  <si>
+    <t>2019/07</t>
+  </si>
+  <si>
+    <t>2024t2</t>
+  </si>
+  <si>
+    <t>2027</t>
+  </si>
+  <si>
+    <t>2011</t>
   </si>
 </sst>
 </file>
@@ -850,7 +859,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -904,7 +913,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -928,10 +937,10 @@
         <v>19</v>
       </c>
       <c r="R1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -939,13 +948,13 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
         <v>123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>124</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -960,7 +969,7 @@
         <v>3000</v>
       </c>
       <c r="K2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L2" s="1">
         <v>2002</v>
@@ -980,13 +989,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -1004,10 +1013,10 @@
         <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>17</v>
@@ -1033,13 +1042,13 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1057,7 +1066,7 @@
         <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1068,10 +1077,10 @@
         <v>22</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1079,7 +1088,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
@@ -1088,7 +1097,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1107,13 +1116,13 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -1122,7 +1131,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1131,7 +1140,7 @@
         <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>43</v>
@@ -1151,7 +1160,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -1166,16 +1175,16 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>49</v>
+        <v>143</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="N7" t="s">
         <v>25</v>
@@ -1186,37 +1195,37 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8">
+        <v>34444</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H8">
-        <v>80000</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="K8" t="s">
+        <v>131</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K8" t="s">
-        <v>132</v>
-      </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="N8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O8" t="s">
         <v>22</v>
@@ -1224,37 +1233,37 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" t="s">
-        <v>57</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9">
         <v>320000</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="K9" t="s">
-        <v>134</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>44</v>
@@ -1268,37 +1277,37 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
         <v>61</v>
-      </c>
-      <c r="B10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" t="s">
-        <v>62</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10">
         <v>67000</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" t="s">
+        <v>132</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="K10" t="s">
-        <v>133</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>44</v>
       </c>
       <c r="N10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O10" t="s">
         <v>22</v>
@@ -1306,31 +1315,31 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" t="s">
         <v>68</v>
-      </c>
-      <c r="B11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" t="s">
-        <v>69</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H11">
-        <v>90000</v>
+        <v>999990</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
+        <v>132</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="K11" t="s">
-        <v>133</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>44</v>
@@ -1344,34 +1353,34 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" t="s">
         <v>72</v>
-      </c>
-      <c r="B12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H12">
         <v>500000</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N12" t="s">
         <v>26</v>
@@ -1380,39 +1389,39 @@
         <v>39</v>
       </c>
       <c r="R12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13">
         <v>200000</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" t="s">
+        <v>133</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K13" t="s">
-        <v>134</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="M13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N13" t="s">
         <v>25</v>
@@ -1423,34 +1432,34 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" t="s">
         <v>80</v>
-      </c>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" t="s">
-        <v>81</v>
       </c>
       <c r="F14" t="s">
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14">
         <v>85000</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="N14" t="s">
         <v>27</v>
@@ -1461,31 +1470,31 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" t="s">
         <v>84</v>
-      </c>
-      <c r="B15" t="s">
-        <v>117</v>
-      </c>
-      <c r="E15" t="s">
-        <v>85</v>
       </c>
       <c r="F15" t="s">
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H15">
         <v>99900</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>44</v>
@@ -1499,31 +1508,31 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" t="s">
-        <v>89</v>
       </c>
       <c r="F16" t="s">
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16">
         <v>250000</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>44</v>
@@ -1537,37 +1546,37 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" t="s">
         <v>92</v>
-      </c>
-      <c r="B17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" t="s">
-        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H17">
         <v>100000</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="N17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O17" t="s">
         <v>22</v>
@@ -1575,31 +1584,31 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
         <v>95</v>
-      </c>
-      <c r="B18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" t="s">
-        <v>96</v>
       </c>
       <c r="F18" t="s">
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H18">
         <v>1300000</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>44</v>
@@ -1613,43 +1622,43 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" t="s">
         <v>98</v>
-      </c>
-      <c r="B19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" t="s">
-        <v>99</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H19">
         <v>46000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="N19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O19" t="s">
         <v>22</v>
@@ -1657,37 +1666,37 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" t="s">
+        <v>133</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="K20" t="s">
-        <v>134</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>44</v>
@@ -1701,34 +1710,34 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" t="s">
         <v>137</v>
-      </c>
-      <c r="B21" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" t="s">
-        <v>138</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21">
         <v>200000</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N21" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
changed : clean up db_schema and remove pdf and use_pdf db fields
</commit_message>
<xml_diff>
--- a/public/data/db_source/dataset.xlsx
+++ b/public/data/db_source/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB2AE4A-1F9D-9A4B-BAF8-C36A8D3E8335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD95C38-FFD6-6F49-9A2F-8276311794FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,9 +325,6 @@
     <t>emploi_jeunes</t>
   </si>
   <si>
-    <t>Données sur l’emploi des jeunes de 18 à 25 ans</t>
-  </si>
-  <si>
     <t>2024/09/10</t>
   </si>
   <si>
@@ -461,6 +458,9 @@
   </si>
   <si>
     <t>2011</t>
+  </si>
+  <si>
+    <t>Données sur l’emploi des jeunes de 18 à 36 ans</t>
   </si>
 </sst>
 </file>
@@ -856,10 +856,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -913,7 +913,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -937,10 +937,10 @@
         <v>19</v>
       </c>
       <c r="R1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -948,13 +948,13 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" t="s">
         <v>122</v>
-      </c>
-      <c r="D2" t="s">
-        <v>123</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -969,7 +969,7 @@
         <v>3000</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L2" s="1">
         <v>2002</v>
@@ -989,13 +989,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
@@ -1013,10 +1013,10 @@
         <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>17</v>
@@ -1042,13 +1042,13 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1066,7 +1066,7 @@
         <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1077,10 +1077,10 @@
         <v>22</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1088,7 +1088,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
@@ -1097,7 +1097,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1116,13 +1116,13 @@
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E6" t="s">
         <v>41</v>
@@ -1131,7 +1131,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1140,7 +1140,7 @@
         <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>43</v>
@@ -1160,7 +1160,7 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -1175,16 +1175,16 @@
         <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="N7" t="s">
         <v>25</v>
@@ -1198,7 +1198,7 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8" t="s">
         <v>50</v>
@@ -1216,7 +1216,7 @@
         <v>52</v>
       </c>
       <c r="K8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>53</v>
@@ -1236,13 +1236,13 @@
         <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
         <v>122</v>
-      </c>
-      <c r="D9" t="s">
-        <v>123</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
@@ -1260,7 +1260,7 @@
         <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>59</v>
@@ -1280,7 +1280,7 @@
         <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
         <v>61</v>
@@ -1298,7 +1298,7 @@
         <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>64</v>
@@ -1318,7 +1318,7 @@
         <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
         <v>68</v>
@@ -1327,7 +1327,7 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H11">
         <v>999990</v>
@@ -1336,7 +1336,7 @@
         <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>70</v>
@@ -1356,7 +1356,7 @@
         <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
         <v>72</v>
@@ -1374,13 +1374,13 @@
         <v>74</v>
       </c>
       <c r="K12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N12" t="s">
         <v>26</v>
@@ -1389,7 +1389,7 @@
         <v>39</v>
       </c>
       <c r="R12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1397,10 +1397,10 @@
         <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -1415,13 +1415,13 @@
         <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>78</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N13" t="s">
         <v>25</v>
@@ -1435,7 +1435,7 @@
         <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" t="s">
         <v>80</v>
@@ -1453,7 +1453,7 @@
         <v>82</v>
       </c>
       <c r="K14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>53</v>
@@ -1473,7 +1473,7 @@
         <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" t="s">
         <v>84</v>
@@ -1491,7 +1491,7 @@
         <v>86</v>
       </c>
       <c r="K15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>70</v>
@@ -1511,7 +1511,7 @@
         <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" t="s">
         <v>88</v>
@@ -1529,7 +1529,7 @@
         <v>90</v>
       </c>
       <c r="K16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>59</v>
@@ -1549,7 +1549,7 @@
         <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
         <v>92</v>
@@ -1558,7 +1558,7 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17">
         <v>100000</v>
@@ -1567,7 +1567,7 @@
         <v>93</v>
       </c>
       <c r="K17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>53</v>
@@ -1587,7 +1587,7 @@
         <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
         <v>95</v>
@@ -1605,10 +1605,10 @@
         <v>69</v>
       </c>
       <c r="K18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>44</v>
@@ -1625,13 +1625,13 @@
         <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E19" t="s">
         <v>98</v>
@@ -1646,16 +1646,16 @@
         <v>46000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>53</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N19" t="s">
         <v>66</v>
@@ -1669,34 +1669,34 @@
         <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="H20">
         <v>100000</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="K20" t="s">
-        <v>133</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>44</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" t="s">
         <v>136</v>
-      </c>
-      <c r="B21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" t="s">
-        <v>137</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -1728,16 +1728,16 @@
         <v>200000</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>78</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N21" t="s">
         <v>25</v>

</xml_diff>